<commit_message>
Test Data user name change - 20 May 2025
</commit_message>
<xml_diff>
--- a/TestData/LV_TMTT0005430_TimeRecorderFunctionalities.xlsx
+++ b/TestData/LV_TMTT0005430_TimeRecorderFunctionalities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F881697-9481-4186-B494-233C33CBC9DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94E41FD-E7FC-4630-BF34-BD42448F685C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="8" r:id="rId1"/>
@@ -115,7 +115,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>Adarsh Patel</t>
+    <t>Aadarsh Patel</t>
   </si>
 </sst>
 </file>

</xml_diff>